<commit_message>
Updated DOB in excel
</commit_message>
<xml_diff>
--- a/src/test/resources/dataFiles/SepsisPatientData.xlsx
+++ b/src/test/resources/dataFiles/SepsisPatientData.xlsx
@@ -166,7 +166,7 @@
     <t>Robert</t>
   </si>
   <si>
-    <t>12/31/2023</t>
+    <t>01/15/2024</t>
   </si>
   <si>
     <t>mrob@gmail.com</t>
@@ -1782,7 +1782,7 @@
         <v>31</v>
       </c>
       <c r="E3" s="7">
-        <v>719645955</v>
+        <v>7196459</v>
       </c>
       <c r="F3" t="s" s="6">
         <v>32</v>

</xml_diff>